<commit_message>
Updated Team Info to include my (Tyler) info.
</commit_message>
<xml_diff>
--- a/Team 44 Info.xlsx
+++ b/Team 44 Info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Course\ComputerScience\Session 5\Agile Software Projects\Github\Project44\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Documents\Projects &amp; Games\Project44\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A453030B-9C47-4940-9F7E-2D7B88B06A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B385A7BB-0ADA-4F52-AEF8-4A6083B211B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A10268F0-EBC9-46C5-894C-FE007EDF445D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A10268F0-EBC9-46C5-894C-FE007EDF445D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -71,6 +71,18 @@
   </si>
   <si>
     <t>UTC+05:30</t>
+  </si>
+  <si>
+    <t>Tyler Dalke</t>
+  </si>
+  <si>
+    <t>TylerADalke22@hotmail.com</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>UTC-5</t>
   </si>
 </sst>
 </file>
@@ -433,21 +445,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A719BD82-4750-4F59-9FC8-DE4A3BC8BD3A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -475,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -487,12 +497,27 @@
       </c>
       <c r="D3" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{5F11463F-3020-4C4D-8D88-7644592C9865}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{9DBA4C49-8364-4FF3-B9BB-C8BF0D0968CD}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{60E2815F-869D-4DDD-B4E1-2249D804ED36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>